<commit_message>
Pradeep temp Area Calender Impliment
</commit_message>
<xml_diff>
--- a/resouces/TestData.xlsx
+++ b/resouces/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRADEEP\eclipse-workspace\PracticeSelenium\resouces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3B62A0-A318-4F09-A1D7-47D7B4C72870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491B8A6E-076E-4063-9728-2D3D4A7A4836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>RUNMODE</t>
   </si>
@@ -57,49 +57,37 @@
     <t>Y</t>
   </si>
   <si>
-    <t>CHROME</t>
-  </si>
-  <si>
-    <t>abcpu</t>
-  </si>
-  <si>
-    <t>pkub</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
     <t>mngr243120</t>
   </si>
   <si>
     <t>udAhydy</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>FIRFOX</t>
-  </si>
-  <si>
-    <t>HJDK44</t>
-  </si>
-  <si>
-    <t>UTGJJG</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>JFJFJF434</t>
-  </si>
-  <si>
-    <t>JFJJGJG44</t>
-  </si>
-  <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t xml:space="preserve"> IE</t>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MozilaFireFox</t>
+  </si>
+  <si>
+    <t>InternetExplore</t>
+  </si>
+  <si>
+    <t>mngrINVALID</t>
+  </si>
+  <si>
+    <t>mng243120</t>
+  </si>
+  <si>
+    <t>INVALID</t>
+  </si>
+  <si>
+    <t>INVALIDJG44</t>
   </si>
 </sst>
 </file>
@@ -433,13 +421,13 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
     <col min="5" max="5" width="17.109375" customWidth="1"/>
@@ -475,13 +463,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -492,16 +480,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -509,16 +497,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -526,16 +514,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>